<commit_message>
Manual Testing Excel Classwork
</commit_message>
<xml_diff>
--- a/Manual Testing.xlsx
+++ b/Manual Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63F1DE4-3FC7-4254-9A52-5DE54610BD2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA9FD15-F2EC-4BFE-B19A-C5EAD50AF5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{37E32107-E032-4525-BEBA-50293EE002C1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t>Project Name:</t>
   </si>
@@ -187,6 +187,40 @@
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>TC_ERP_Login_003</t>
+  </si>
+  <si>
+    <t>Enter a invalid username &amp; an valid password</t>
+  </si>
+  <si>
+    <t>1. Enter invalid username
+2. Enter valid password
+3. Click on the login button</t>
+  </si>
+  <si>
+    <t>Username:
+xxxxx@erp.com
+Password:
+P@ssw0rd</t>
+  </si>
+  <si>
+    <t>TC_ERP_Login_004</t>
+  </si>
+  <si>
+    <t>Enter a invalid username &amp; an invalid password</t>
+  </si>
+  <si>
+    <t>1. Enter invalid username
+2. Enter invalid password
+3. Click on the login button</t>
+  </si>
+  <si>
+    <t>Username:
+xxxxx@erp.com
+Password:
+xxxxxxxx</t>
   </si>
 </sst>
 </file>
@@ -196,7 +230,7 @@
   <numFmts count="1">
     <numFmt numFmtId="166" formatCode="ddd\,/dd\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,16 +238,70 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -221,27 +309,240 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -557,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E1E475-AD56-4218-B114-741CF0C8EB68}">
-  <dimension ref="A2:R15"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -569,7 +870,7 @@
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6328125" customWidth="1"/>
-    <col min="5" max="5" width="13.08984375" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" customWidth="1"/>
     <col min="6" max="6" width="8.81640625" customWidth="1"/>
     <col min="7" max="7" width="15.26953125" customWidth="1"/>
     <col min="8" max="8" width="9.36328125" customWidth="1"/>
@@ -581,194 +882,282 @@
     <col min="14" max="14" width="10" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="8">
         <v>44741</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="7" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="9">
         <v>44765</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+    <row r="8" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="1:18" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="N9" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:18" s="2" customFormat="1" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="15">
         <v>44748</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="N10" s="17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:18" s="4" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:18" s="2" customFormat="1" ht="102" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="12">
         <v>44750</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="N11" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:18" s="2" customFormat="1" ht="102" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="M12" s="15">
+        <v>44752</v>
+      </c>
+      <c r="N12" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" s="2" customFormat="1" ht="102" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13" s="12">
+        <v>44757</v>
+      </c>
+      <c r="N13" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>

</xml_diff>